<commit_message>
code to genarated the random data from the excel
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/RestAssured.xlsx
+++ b/src/test/resources/TestData/RestAssured.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESoft_Solutions\API_Testing\RestAssuredFrameWork\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESoft_Solutions\API_Testing\RestAssured_DataDriven\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4E486A-C7E4-414F-8DF3-0F42C761B349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE085597-A08A-4911-BB29-CBCE105C45B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>BaseUrl</t>
   </si>
@@ -53,56 +53,43 @@
     <t>Post</t>
   </si>
   <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Basepath</t>
+  </si>
+  <si>
+    <t>PathParameters</t>
+  </si>
+  <si>
+    <t>users/1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>pass or fail</t>
+  </si>
+  <si>
     <t>{
-    "createdAt": "2024-05-03T04:02:05.445Z",
-    "name": "Arlene Bauch",
-    "email": "Bridie76@example.net",
-    "given_name": "Alisa",
-    "last_ip": "152.159.43.27",
-    "updated_at": "2074-07-25T22:41:34.935Z",
-    "last_login": "2023-08-12T19:30:20.370Z",
-    "email_verified": false
-  }</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>Get</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Put</t>
-  </si>
-  <si>
-    <t>{
-    "createdAt": "2024-05-03T04:02:05.445Z",
-    "name": "Gopi Bauch",
-    "email": "gopi@example.net",
-    "given_name": "Alisa",
-    "last_ip": "152.159.43.27",
-    "updated_at": "2074-07-25T22:41:34.935Z",
-    "last_login": "2023-08-12T19:30:20.370Z",
-    "email_verified": false,
-    "user_id": "1"
-  }</t>
-  </si>
-  <si>
-    <t>Basepath</t>
-  </si>
-  <si>
-    <t>PathParameters</t>
-  </si>
-  <si>
-    <t>users/1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>pass or fail</t>
+  "createdAt": "$RandomPastDate",
+  "name": "$RandomFullName",
+  "email": "$RandomEmail",
+  "given_name": "$RandomFirstName",
+  "last_ip": "$RandomComputerIP",
+  "updated_at": "$RandomPastDate",
+  "last_login": "$RandomFutureDate",
+  "email_verified": "$RandomBooleanValue"
+}</t>
   </si>
 </sst>
 </file>
@@ -487,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0268B1-42EB-49EC-8577-C6340322AACE}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,10 +495,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -526,7 +513,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="145" x14ac:dyDescent="0.35">
@@ -543,10 +530,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="H2"/>
     </row>
@@ -561,11 +548,11 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -573,37 +560,37 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -632,7 +619,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated else block in randomRequestJsonObject
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/RestAssured.xlsx
+++ b/src/test/resources/TestData/RestAssured.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESoft_Solutions\API_Testing\RestAssured_DataDriven\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE085597-A08A-4911-BB29-CBCE105C45B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25050EB4-FB5D-4FA6-B9C6-8DF1E5509181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>BaseUrl</t>
   </si>
@@ -83,6 +83,18 @@
     <t>{
   "createdAt": "$RandomPastDate",
   "name": "$RandomFullName",
+  "email": "$RandomEmail",
+  "given_name": "$RandomFirstName",
+  "last_ip": "$RandomComputerIP",
+  "updated_at": "$RandomPastDate",
+  "last_login": "$RandomFutureDate",
+  "email_verified": "$RandomBooleanValue"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "createdAt": "$RandomPastDate",
+  "name": "Gopi Appapuram",
   "email": "$RandomEmail",
   "given_name": "$RandomFirstName",
   "last_ip": "$RandomComputerIP",
@@ -474,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0268B1-42EB-49EC-8577-C6340322AACE}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +542,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>

</xml_diff>